<commit_message>
correct unit test for dao layer
</commit_message>
<xml_diff>
--- a/src/test/resources/com/ian/sblog/dao/test.Users.xlsx
+++ b/src/test/resources/com/ian/sblog/dao/test.Users.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16944" windowHeight="2364"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16944" windowHeight="4272"/>
   </bookViews>
   <sheets>
     <sheet name="bg_user" sheetId="1" r:id="rId1"/>
@@ -46,19 +46,19 @@
     <t>Kaka Ian</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>USERNAME</t>
-  </si>
-  <si>
-    <t>PASSWORD</t>
-  </si>
-  <si>
-    <t>DISPLAY_NAME</t>
-  </si>
-  <si>
-    <t>REAL_NAME</t>
+    <t>id</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>display_name</t>
+  </si>
+  <si>
+    <t>real_name</t>
   </si>
 </sst>
 </file>

</xml_diff>